<commit_message>
keeping up to date
</commit_message>
<xml_diff>
--- a/Analisis.xlsx
+++ b/Analisis.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H154"/>
+  <dimension ref="A1:H173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5068,6 +5068,576 @@
       </c>
       <c r="H154" t="n">
         <v>9.800000000000001</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Getafe</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>0</v>
+      </c>
+      <c r="D155" t="n">
+        <v>0</v>
+      </c>
+      <c r="E155" t="n">
+        <v>2.007</v>
+      </c>
+      <c r="F155" t="n">
+        <v>1.443</v>
+      </c>
+      <c r="G155" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="H155" t="n">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Villarreal</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Celta Vigo</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>1</v>
+      </c>
+      <c r="D156" t="n">
+        <v>0</v>
+      </c>
+      <c r="E156" t="n">
+        <v>1.667</v>
+      </c>
+      <c r="F156" t="n">
+        <v>0.9379999999999999</v>
+      </c>
+      <c r="G156" t="n">
+        <v>54.52</v>
+      </c>
+      <c r="H156" t="n">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Granada</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Elche</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>0</v>
+      </c>
+      <c r="D157" t="n">
+        <v>1</v>
+      </c>
+      <c r="E157" t="n">
+        <v>1.711</v>
+      </c>
+      <c r="F157" t="n">
+        <v>1.462</v>
+      </c>
+      <c r="G157" t="n">
+        <v>33</v>
+      </c>
+      <c r="H157" t="n">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Levante</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Espanyol</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>1</v>
+      </c>
+      <c r="D158" t="n">
+        <v>1</v>
+      </c>
+      <c r="E158" t="n">
+        <v>1.843</v>
+      </c>
+      <c r="F158" t="n">
+        <v>1.526</v>
+      </c>
+      <c r="G158" t="n">
+        <v>22.48</v>
+      </c>
+      <c r="H158" t="n">
+        <v>9.699999999999999</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Osasuna</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>4</v>
+      </c>
+      <c r="D159" t="n">
+        <v>0</v>
+      </c>
+      <c r="E159" t="n">
+        <v>1.582</v>
+      </c>
+      <c r="F159" t="n">
+        <v>1.278</v>
+      </c>
+      <c r="G159" t="n">
+        <v>44.48</v>
+      </c>
+      <c r="H159" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Real Sociedad</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Alaves</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>1</v>
+      </c>
+      <c r="D160" t="n">
+        <v>0</v>
+      </c>
+      <c r="E160" t="n">
+        <v>1.334</v>
+      </c>
+      <c r="F160" t="n">
+        <v>0.381</v>
+      </c>
+      <c r="G160" t="n">
+        <v>61.12</v>
+      </c>
+      <c r="H160" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Betis</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Ath. Bilbao</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>1</v>
+      </c>
+      <c r="D161" t="n">
+        <v>0</v>
+      </c>
+      <c r="E161" t="n">
+        <v>1.314</v>
+      </c>
+      <c r="F161" t="n">
+        <v>0.965</v>
+      </c>
+      <c r="G161" t="n">
+        <v>44.62</v>
+      </c>
+      <c r="H161" t="n">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Vallecano</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Sevilla</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>1</v>
+      </c>
+      <c r="D162" t="n">
+        <v>1</v>
+      </c>
+      <c r="E162" t="n">
+        <v>0.545</v>
+      </c>
+      <c r="F162" t="n">
+        <v>0.591</v>
+      </c>
+      <c r="G162" t="n">
+        <v>43.32</v>
+      </c>
+      <c r="H162" t="n">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Mallorca</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Real Madryt</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>0</v>
+      </c>
+      <c r="D163" t="n">
+        <v>3</v>
+      </c>
+      <c r="E163" t="n">
+        <v>0.624</v>
+      </c>
+      <c r="F163" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="G163" t="n">
+        <v>68.48999999999999</v>
+      </c>
+      <c r="H163" t="n">
+        <v>9.300000000000001</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Ath. Bilbao</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Getafe</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>1</v>
+      </c>
+      <c r="D164" t="n">
+        <v>1</v>
+      </c>
+      <c r="E164" t="n">
+        <v>1.909</v>
+      </c>
+      <c r="F164" t="n">
+        <v>0.597</v>
+      </c>
+      <c r="G164" t="n">
+        <v>20.47</v>
+      </c>
+      <c r="H164" t="n">
+        <v>9.300000000000001</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Vallecano</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Atl. Madryt</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>0</v>
+      </c>
+      <c r="D165" t="n">
+        <v>1</v>
+      </c>
+      <c r="E165" t="n">
+        <v>1.732</v>
+      </c>
+      <c r="F165" t="n">
+        <v>1.566</v>
+      </c>
+      <c r="G165" t="n">
+        <v>35.03</v>
+      </c>
+      <c r="H165" t="n">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Osasuna</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Levante</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>3</v>
+      </c>
+      <c r="D166" t="n">
+        <v>1</v>
+      </c>
+      <c r="E166" t="n">
+        <v>1.353</v>
+      </c>
+      <c r="F166" t="n">
+        <v>1.308</v>
+      </c>
+      <c r="G166" t="n">
+        <v>38.03</v>
+      </c>
+      <c r="H166" t="n">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Elche</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>0</v>
+      </c>
+      <c r="D167" t="n">
+        <v>1</v>
+      </c>
+      <c r="E167" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="F167" t="n">
+        <v>1.488</v>
+      </c>
+      <c r="G167" t="n">
+        <v>35.17</v>
+      </c>
+      <c r="H167" t="n">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Alaves</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Granada</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>2</v>
+      </c>
+      <c r="D168" t="n">
+        <v>3</v>
+      </c>
+      <c r="E168" t="n">
+        <v>0.872</v>
+      </c>
+      <c r="F168" t="n">
+        <v>0.8179999999999999</v>
+      </c>
+      <c r="G168" t="n">
+        <v>31.41</v>
+      </c>
+      <c r="H168" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Real Madryt</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>0</v>
+      </c>
+      <c r="D169" t="n">
+        <v>4</v>
+      </c>
+      <c r="E169" t="n">
+        <v>1.979</v>
+      </c>
+      <c r="F169" t="n">
+        <v>0.997</v>
+      </c>
+      <c r="G169" t="n">
+        <v>18.45</v>
+      </c>
+      <c r="H169" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Sevilla</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Real Sociedad</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>0</v>
+      </c>
+      <c r="D170" t="n">
+        <v>0</v>
+      </c>
+      <c r="E170" t="n">
+        <v>2.703</v>
+      </c>
+      <c r="F170" t="n">
+        <v>1.027</v>
+      </c>
+      <c r="G170" t="n">
+        <v>15.38</v>
+      </c>
+      <c r="H170" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Celta Vigo</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Betis</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>0</v>
+      </c>
+      <c r="D171" t="n">
+        <v>0</v>
+      </c>
+      <c r="E171" t="n">
+        <v>1.325</v>
+      </c>
+      <c r="F171" t="n">
+        <v>2.424</v>
+      </c>
+      <c r="G171" t="n">
+        <v>18.65</v>
+      </c>
+      <c r="H171" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Cadiz</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Villarreal</t>
+        </is>
+      </c>
+      <c r="C172" t="n">
+        <v>1</v>
+      </c>
+      <c r="D172" t="n">
+        <v>0</v>
+      </c>
+      <c r="E172" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="F172" t="n">
+        <v>1.313</v>
+      </c>
+      <c r="G172" t="n">
+        <v>16.18</v>
+      </c>
+      <c r="H172" t="n">
+        <v>8.699999999999999</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Espanyol</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Mallorca</t>
+        </is>
+      </c>
+      <c r="C173" t="n">
+        <v>1</v>
+      </c>
+      <c r="D173" t="n">
+        <v>0</v>
+      </c>
+      <c r="E173" t="n">
+        <v>2.736</v>
+      </c>
+      <c r="F173" t="n">
+        <v>1.174</v>
+      </c>
+      <c r="G173" t="n">
+        <v>70.22</v>
+      </c>
+      <c r="H173" t="n">
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -9162,7 +9732,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H172"/>
+  <dimension ref="A1:H189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14340,6 +14910,516 @@
       </c>
       <c r="H172" t="n">
         <v>4.4</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Manchester Utd</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Tottenham</t>
+        </is>
+      </c>
+      <c r="C173" t="n">
+        <v>3</v>
+      </c>
+      <c r="D173" t="n">
+        <v>2</v>
+      </c>
+      <c r="E173" t="n">
+        <v>1.434</v>
+      </c>
+      <c r="F173" t="n">
+        <v>1.313</v>
+      </c>
+      <c r="G173" t="n">
+        <v>40.01</v>
+      </c>
+      <c r="H173" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Burnley</t>
+        </is>
+      </c>
+      <c r="C174" t="n">
+        <v>2</v>
+      </c>
+      <c r="D174" t="n">
+        <v>0</v>
+      </c>
+      <c r="E174" t="n">
+        <v>1.036</v>
+      </c>
+      <c r="F174" t="n">
+        <v>1.089</v>
+      </c>
+      <c r="G174" t="n">
+        <v>33.78</v>
+      </c>
+      <c r="H174" t="n">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Brighton</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>0</v>
+      </c>
+      <c r="D175" t="n">
+        <v>2</v>
+      </c>
+      <c r="E175" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="F175" t="n">
+        <v>2.731</v>
+      </c>
+      <c r="G175" t="n">
+        <v>83.73999999999999</v>
+      </c>
+      <c r="H175" t="n">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Leicester</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>2</v>
+      </c>
+      <c r="D176" t="n">
+        <v>0</v>
+      </c>
+      <c r="E176" t="n">
+        <v>2.532</v>
+      </c>
+      <c r="F176" t="n">
+        <v>0.986</v>
+      </c>
+      <c r="G176" t="n">
+        <v>70.88</v>
+      </c>
+      <c r="H176" t="n">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>West Ham</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Aston Villa</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>2</v>
+      </c>
+      <c r="D177" t="n">
+        <v>1</v>
+      </c>
+      <c r="E177" t="n">
+        <v>1.501</v>
+      </c>
+      <c r="F177" t="n">
+        <v>1.327</v>
+      </c>
+      <c r="G177" t="n">
+        <v>41.41</v>
+      </c>
+      <c r="H177" t="n">
+        <v>8.800000000000001</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Southampton</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Watford</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
+        <v>1</v>
+      </c>
+      <c r="D178" t="n">
+        <v>2</v>
+      </c>
+      <c r="E178" t="n">
+        <v>1.471</v>
+      </c>
+      <c r="F178" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="G178" t="n">
+        <v>16.66</v>
+      </c>
+      <c r="H178" t="n">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Leeds</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>2</v>
+      </c>
+      <c r="D179" t="n">
+        <v>1</v>
+      </c>
+      <c r="E179" t="n">
+        <v>1.794</v>
+      </c>
+      <c r="F179" t="n">
+        <v>0.966</v>
+      </c>
+      <c r="G179" t="n">
+        <v>56.84</v>
+      </c>
+      <c r="H179" t="n">
+        <v>9.800000000000001</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Wolves</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>0</v>
+      </c>
+      <c r="D180" t="n">
+        <v>1</v>
+      </c>
+      <c r="E180" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="F180" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G180" t="n">
+        <v>45.71</v>
+      </c>
+      <c r="H180" t="n">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
+        <v>1</v>
+      </c>
+      <c r="D181" t="n">
+        <v>0</v>
+      </c>
+      <c r="E181" t="n">
+        <v>2.605</v>
+      </c>
+      <c r="F181" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="G181" t="n">
+        <v>78.88</v>
+      </c>
+      <c r="H181" t="n">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Crystal Palace</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Manchester City</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>0</v>
+      </c>
+      <c r="D182" t="n">
+        <v>0</v>
+      </c>
+      <c r="E182" t="n">
+        <v>0.607</v>
+      </c>
+      <c r="F182" t="n">
+        <v>1.965</v>
+      </c>
+      <c r="G182" t="n">
+        <v>19.85</v>
+      </c>
+      <c r="H182" t="n">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
+        <v>0</v>
+      </c>
+      <c r="D183" t="n">
+        <v>2</v>
+      </c>
+      <c r="E183" t="n">
+        <v>1.145</v>
+      </c>
+      <c r="F183" t="n">
+        <v>1.549</v>
+      </c>
+      <c r="G183" t="n">
+        <v>46.63</v>
+      </c>
+      <c r="H183" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Brighton</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Tottenham</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>0</v>
+      </c>
+      <c r="D184" t="n">
+        <v>2</v>
+      </c>
+      <c r="E184" t="n">
+        <v>0.747</v>
+      </c>
+      <c r="F184" t="n">
+        <v>1.724</v>
+      </c>
+      <c r="G184" t="n">
+        <v>60.76</v>
+      </c>
+      <c r="H184" t="n">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>1</v>
+      </c>
+      <c r="D185" t="n">
+        <v>0</v>
+      </c>
+      <c r="E185" t="n">
+        <v>1.593</v>
+      </c>
+      <c r="F185" t="n">
+        <v>1.124</v>
+      </c>
+      <c r="G185" t="n">
+        <v>48.22</v>
+      </c>
+      <c r="H185" t="n">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Wolves</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Leeds</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>2</v>
+      </c>
+      <c r="D186" t="n">
+        <v>3</v>
+      </c>
+      <c r="E186" t="n">
+        <v>2.072</v>
+      </c>
+      <c r="F186" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="G186" t="n">
+        <v>11.73</v>
+      </c>
+      <c r="H186" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Aston Villa</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
+        <v>0</v>
+      </c>
+      <c r="D187" t="n">
+        <v>1</v>
+      </c>
+      <c r="E187" t="n">
+        <v>2.133</v>
+      </c>
+      <c r="F187" t="n">
+        <v>2</v>
+      </c>
+      <c r="G187" t="n">
+        <v>37.33</v>
+      </c>
+      <c r="H187" t="n">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Tottenham</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>West Ham</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>3</v>
+      </c>
+      <c r="D188" t="n">
+        <v>1</v>
+      </c>
+      <c r="E188" t="n">
+        <v>1.484</v>
+      </c>
+      <c r="F188" t="n">
+        <v>1.338</v>
+      </c>
+      <c r="G188" t="n">
+        <v>40.75</v>
+      </c>
+      <c r="H188" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Leicester</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>2</v>
+      </c>
+      <c r="D189" t="n">
+        <v>1</v>
+      </c>
+      <c r="E189" t="n">
+        <v>2.221</v>
+      </c>
+      <c r="F189" t="n">
+        <v>1.316</v>
+      </c>
+      <c r="G189" t="n">
+        <v>57.92</v>
+      </c>
+      <c r="H189" t="n">
+        <v>9.4</v>
       </c>
     </row>
   </sheetData>
@@ -14353,7 +15433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H232"/>
+  <dimension ref="A1:H252"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21331,6 +22411,606 @@
       </c>
       <c r="H232" t="n">
         <v>2.6</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Bournemouth</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Reading</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>1</v>
+      </c>
+      <c r="D233" t="n">
+        <v>1</v>
+      </c>
+      <c r="E233" t="n">
+        <v>2.931</v>
+      </c>
+      <c r="F233" t="n">
+        <v>1.085</v>
+      </c>
+      <c r="G233" t="n">
+        <v>14.07</v>
+      </c>
+      <c r="H233" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Blackburn</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Derby</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>3</v>
+      </c>
+      <c r="D234" t="n">
+        <v>1</v>
+      </c>
+      <c r="E234" t="n">
+        <v>1.688</v>
+      </c>
+      <c r="F234" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="G234" t="n">
+        <v>63.99</v>
+      </c>
+      <c r="H234" t="n">
+        <v>4.9</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Birmingham</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Middlesbrough</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
+        <v>0</v>
+      </c>
+      <c r="D235" t="n">
+        <v>2</v>
+      </c>
+      <c r="E235" t="n">
+        <v>1.388</v>
+      </c>
+      <c r="F235" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="G235" t="n">
+        <v>36.84</v>
+      </c>
+      <c r="H235" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Barnsley</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Bristol City</t>
+        </is>
+      </c>
+      <c r="C236" t="n">
+        <v>2</v>
+      </c>
+      <c r="D236" t="n">
+        <v>0</v>
+      </c>
+      <c r="E236" t="n">
+        <v>1.431</v>
+      </c>
+      <c r="F236" t="n">
+        <v>1.464</v>
+      </c>
+      <c r="G236" t="n">
+        <v>36.86</v>
+      </c>
+      <c r="H236" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Peterborough</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Swansea</t>
+        </is>
+      </c>
+      <c r="C237" t="n">
+        <v>2</v>
+      </c>
+      <c r="D237" t="n">
+        <v>3</v>
+      </c>
+      <c r="E237" t="n">
+        <v>1.193</v>
+      </c>
+      <c r="F237" t="n">
+        <v>1.158</v>
+      </c>
+      <c r="G237" t="n">
+        <v>35.15</v>
+      </c>
+      <c r="H237" t="n">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Nottingham</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>QPR</t>
+        </is>
+      </c>
+      <c r="C238" t="n">
+        <v>3</v>
+      </c>
+      <c r="D238" t="n">
+        <v>1</v>
+      </c>
+      <c r="E238" t="n">
+        <v>1.509</v>
+      </c>
+      <c r="F238" t="n">
+        <v>1.553</v>
+      </c>
+      <c r="G238" t="n">
+        <v>37.03</v>
+      </c>
+      <c r="H238" t="n">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Millwall</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Huddersfield</t>
+        </is>
+      </c>
+      <c r="C239" t="n">
+        <v>2</v>
+      </c>
+      <c r="D239" t="n">
+        <v>0</v>
+      </c>
+      <c r="E239" t="n">
+        <v>1.031</v>
+      </c>
+      <c r="F239" t="n">
+        <v>0.954</v>
+      </c>
+      <c r="G239" t="n">
+        <v>36.54</v>
+      </c>
+      <c r="H239" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Luton</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Preston</t>
+        </is>
+      </c>
+      <c r="C240" t="n">
+        <v>4</v>
+      </c>
+      <c r="D240" t="n">
+        <v>0</v>
+      </c>
+      <c r="E240" t="n">
+        <v>1.255</v>
+      </c>
+      <c r="F240" t="n">
+        <v>0.834</v>
+      </c>
+      <c r="G240" t="n">
+        <v>46.16</v>
+      </c>
+      <c r="H240" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Coventry</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Hull</t>
+        </is>
+      </c>
+      <c r="C241" t="n">
+        <v>0</v>
+      </c>
+      <c r="D241" t="n">
+        <v>2</v>
+      </c>
+      <c r="E241" t="n">
+        <v>1.083</v>
+      </c>
+      <c r="F241" t="n">
+        <v>0.766</v>
+      </c>
+      <c r="G241" t="n">
+        <v>25.59</v>
+      </c>
+      <c r="H241" t="n">
+        <v>4.6</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Cardiff</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Stoke</t>
+        </is>
+      </c>
+      <c r="C242" t="n">
+        <v>2</v>
+      </c>
+      <c r="D242" t="n">
+        <v>1</v>
+      </c>
+      <c r="E242" t="n">
+        <v>0.907</v>
+      </c>
+      <c r="F242" t="n">
+        <v>1.265</v>
+      </c>
+      <c r="G242" t="n">
+        <v>26.63</v>
+      </c>
+      <c r="H242" t="n">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Blackpool</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Sheffield Utd</t>
+        </is>
+      </c>
+      <c r="C243" t="n">
+        <v>0</v>
+      </c>
+      <c r="D243" t="n">
+        <v>0</v>
+      </c>
+      <c r="E243" t="n">
+        <v>1.135</v>
+      </c>
+      <c r="F243" t="n">
+        <v>1.098</v>
+      </c>
+      <c r="G243" t="n">
+        <v>28.87</v>
+      </c>
+      <c r="H243" t="n">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Swansea</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Birmingham</t>
+        </is>
+      </c>
+      <c r="C244" t="n">
+        <v>0</v>
+      </c>
+      <c r="D244" t="n">
+        <v>0</v>
+      </c>
+      <c r="E244" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="F244" t="n">
+        <v>1.365</v>
+      </c>
+      <c r="G244" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="H244" t="n">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Stoke</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Millwall</t>
+        </is>
+      </c>
+      <c r="C245" t="n">
+        <v>2</v>
+      </c>
+      <c r="D245" t="n">
+        <v>0</v>
+      </c>
+      <c r="E245" t="n">
+        <v>1.188</v>
+      </c>
+      <c r="F245" t="n">
+        <v>1.057</v>
+      </c>
+      <c r="G245" t="n">
+        <v>38.92</v>
+      </c>
+      <c r="H245" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Reading</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Blackburn</t>
+        </is>
+      </c>
+      <c r="C246" t="n">
+        <v>1</v>
+      </c>
+      <c r="D246" t="n">
+        <v>0</v>
+      </c>
+      <c r="E246" t="n">
+        <v>1.009</v>
+      </c>
+      <c r="F246" t="n">
+        <v>1.467</v>
+      </c>
+      <c r="G246" t="n">
+        <v>25.99</v>
+      </c>
+      <c r="H246" t="n">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Hull</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Luton</t>
+        </is>
+      </c>
+      <c r="C247" t="n">
+        <v>1</v>
+      </c>
+      <c r="D247" t="n">
+        <v>3</v>
+      </c>
+      <c r="E247" t="n">
+        <v>0.757</v>
+      </c>
+      <c r="F247" t="n">
+        <v>1.478</v>
+      </c>
+      <c r="G247" t="n">
+        <v>54.37</v>
+      </c>
+      <c r="H247" t="n">
+        <v>4.4</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Huddersfield</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Bournemouth</t>
+        </is>
+      </c>
+      <c r="C248" t="n">
+        <v>0</v>
+      </c>
+      <c r="D248" t="n">
+        <v>3</v>
+      </c>
+      <c r="E248" t="n">
+        <v>0.905</v>
+      </c>
+      <c r="F248" t="n">
+        <v>1.115</v>
+      </c>
+      <c r="G248" t="n">
+        <v>40.25</v>
+      </c>
+      <c r="H248" t="n">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Bristol City</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>West Brom</t>
+        </is>
+      </c>
+      <c r="C249" t="n">
+        <v>2</v>
+      </c>
+      <c r="D249" t="n">
+        <v>2</v>
+      </c>
+      <c r="E249" t="n">
+        <v>1.103</v>
+      </c>
+      <c r="F249" t="n">
+        <v>1.131</v>
+      </c>
+      <c r="G249" t="n">
+        <v>28.86</v>
+      </c>
+      <c r="H249" t="n">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Sheffield Utd</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Barnsley</t>
+        </is>
+      </c>
+      <c r="C250" t="n">
+        <v>2</v>
+      </c>
+      <c r="D250" t="n">
+        <v>0</v>
+      </c>
+      <c r="E250" t="n">
+        <v>2.275</v>
+      </c>
+      <c r="F250" t="n">
+        <v>0.515</v>
+      </c>
+      <c r="G250" t="n">
+        <v>77.45</v>
+      </c>
+      <c r="H250" t="n">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Derby</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Coventry</t>
+        </is>
+      </c>
+      <c r="C251" t="n">
+        <v>1</v>
+      </c>
+      <c r="D251" t="n">
+        <v>1</v>
+      </c>
+      <c r="E251" t="n">
+        <v>1.645</v>
+      </c>
+      <c r="F251" t="n">
+        <v>0.996</v>
+      </c>
+      <c r="G251" t="n">
+        <v>24.56</v>
+      </c>
+      <c r="H251" t="n">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>QPR</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Peterborough</t>
+        </is>
+      </c>
+      <c r="C252" t="n">
+        <v>1</v>
+      </c>
+      <c r="D252" t="n">
+        <v>3</v>
+      </c>
+      <c r="E252" t="n">
+        <v>2.808</v>
+      </c>
+      <c r="F252" t="n">
+        <v>0.485</v>
+      </c>
+      <c r="G252" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="H252" t="n">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -21344,7 +23024,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H166"/>
+  <dimension ref="A1:H186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26342,6 +28022,606 @@
       </c>
       <c r="H166" t="n">
         <v>12.6</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>AC Milan</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Empoli</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>1</v>
+      </c>
+      <c r="D167" t="n">
+        <v>0</v>
+      </c>
+      <c r="E167" t="n">
+        <v>1.244</v>
+      </c>
+      <c r="F167" t="n">
+        <v>0.8149999999999999</v>
+      </c>
+      <c r="G167" t="n">
+        <v>46.32</v>
+      </c>
+      <c r="H167" t="n">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Sampdoria</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>1</v>
+      </c>
+      <c r="D168" t="n">
+        <v>3</v>
+      </c>
+      <c r="E168" t="n">
+        <v>1.336</v>
+      </c>
+      <c r="F168" t="n">
+        <v>2.329</v>
+      </c>
+      <c r="G168" t="n">
+        <v>59.62</v>
+      </c>
+      <c r="H168" t="n">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Spezia</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>2</v>
+      </c>
+      <c r="D169" t="n">
+        <v>0</v>
+      </c>
+      <c r="E169" t="n">
+        <v>1.281</v>
+      </c>
+      <c r="F169" t="n">
+        <v>0.958</v>
+      </c>
+      <c r="G169" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="H169" t="n">
+        <v>8.699999999999999</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Salernitana</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Sassuolo</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>2</v>
+      </c>
+      <c r="D170" t="n">
+        <v>2</v>
+      </c>
+      <c r="E170" t="n">
+        <v>1.049</v>
+      </c>
+      <c r="F170" t="n">
+        <v>3.858</v>
+      </c>
+      <c r="G170" t="n">
+        <v>8.529999999999999</v>
+      </c>
+      <c r="H170" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Inter</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>1</v>
+      </c>
+      <c r="D171" t="n">
+        <v>1</v>
+      </c>
+      <c r="E171" t="n">
+        <v>0.979</v>
+      </c>
+      <c r="F171" t="n">
+        <v>1.628</v>
+      </c>
+      <c r="G171" t="n">
+        <v>24.73</v>
+      </c>
+      <c r="H171" t="n">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Udinese</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>AS Roma</t>
+        </is>
+      </c>
+      <c r="C172" t="n">
+        <v>1</v>
+      </c>
+      <c r="D172" t="n">
+        <v>1</v>
+      </c>
+      <c r="E172" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F172" t="n">
+        <v>2.372</v>
+      </c>
+      <c r="G172" t="n">
+        <v>19.35</v>
+      </c>
+      <c r="H172" t="n">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="C173" t="n">
+        <v>0</v>
+      </c>
+      <c r="D173" t="n">
+        <v>0</v>
+      </c>
+      <c r="E173" t="n">
+        <v>2.615</v>
+      </c>
+      <c r="F173" t="n">
+        <v>1</v>
+      </c>
+      <c r="G173" t="n">
+        <v>15.91</v>
+      </c>
+      <c r="H173" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Verona</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="C174" t="n">
+        <v>1</v>
+      </c>
+      <c r="D174" t="n">
+        <v>2</v>
+      </c>
+      <c r="E174" t="n">
+        <v>1.136</v>
+      </c>
+      <c r="F174" t="n">
+        <v>1.825</v>
+      </c>
+      <c r="G174" t="n">
+        <v>53.49</v>
+      </c>
+      <c r="H174" t="n">
+        <v>9.800000000000001</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Fiorentina</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>1</v>
+      </c>
+      <c r="D175" t="n">
+        <v>0</v>
+      </c>
+      <c r="E175" t="n">
+        <v>3.209</v>
+      </c>
+      <c r="F175" t="n">
+        <v>1.001</v>
+      </c>
+      <c r="G175" t="n">
+        <v>80.08</v>
+      </c>
+      <c r="H175" t="n">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Venezia</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>1</v>
+      </c>
+      <c r="D176" t="n">
+        <v>0</v>
+      </c>
+      <c r="E176" t="n">
+        <v>3.118</v>
+      </c>
+      <c r="F176" t="n">
+        <v>0.874</v>
+      </c>
+      <c r="G176" t="n">
+        <v>81.3</v>
+      </c>
+      <c r="H176" t="n">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>1</v>
+      </c>
+      <c r="D177" t="n">
+        <v>0</v>
+      </c>
+      <c r="E177" t="n">
+        <v>0.446</v>
+      </c>
+      <c r="F177" t="n">
+        <v>0.5659999999999999</v>
+      </c>
+      <c r="G177" t="n">
+        <v>22.92</v>
+      </c>
+      <c r="H177" t="n">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Sassuolo</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Spezia</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
+        <v>4</v>
+      </c>
+      <c r="D178" t="n">
+        <v>1</v>
+      </c>
+      <c r="E178" t="n">
+        <v>2.144</v>
+      </c>
+      <c r="F178" t="n">
+        <v>1.224</v>
+      </c>
+      <c r="G178" t="n">
+        <v>58.39</v>
+      </c>
+      <c r="H178" t="n">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>AC Milan</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>0</v>
+      </c>
+      <c r="D179" t="n">
+        <v>1</v>
+      </c>
+      <c r="E179" t="n">
+        <v>0.957</v>
+      </c>
+      <c r="F179" t="n">
+        <v>3.228</v>
+      </c>
+      <c r="G179" t="n">
+        <v>81.08</v>
+      </c>
+      <c r="H179" t="n">
+        <v>4.9</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Inter</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Fiorentina</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>1</v>
+      </c>
+      <c r="D180" t="n">
+        <v>1</v>
+      </c>
+      <c r="E180" t="n">
+        <v>2.675</v>
+      </c>
+      <c r="F180" t="n">
+        <v>0.751</v>
+      </c>
+      <c r="G180" t="n">
+        <v>13.9</v>
+      </c>
+      <c r="H180" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Udinese</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
+        <v>2</v>
+      </c>
+      <c r="D181" t="n">
+        <v>1</v>
+      </c>
+      <c r="E181" t="n">
+        <v>2.034</v>
+      </c>
+      <c r="F181" t="n">
+        <v>0.678</v>
+      </c>
+      <c r="G181" t="n">
+        <v>69.18000000000001</v>
+      </c>
+      <c r="H181" t="n">
+        <v>9.300000000000001</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>0</v>
+      </c>
+      <c r="D182" t="n">
+        <v>1</v>
+      </c>
+      <c r="E182" t="n">
+        <v>0.847</v>
+      </c>
+      <c r="F182" t="n">
+        <v>1.689</v>
+      </c>
+      <c r="G182" t="n">
+        <v>57.34</v>
+      </c>
+      <c r="H182" t="n">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>AS Roma</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
+        <v>3</v>
+      </c>
+      <c r="D183" t="n">
+        <v>0</v>
+      </c>
+      <c r="E183" t="n">
+        <v>1.486</v>
+      </c>
+      <c r="F183" t="n">
+        <v>1.253</v>
+      </c>
+      <c r="G183" t="n">
+        <v>42.62</v>
+      </c>
+      <c r="H183" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Salernitana</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>2</v>
+      </c>
+      <c r="D184" t="n">
+        <v>0</v>
+      </c>
+      <c r="E184" t="n">
+        <v>2.247</v>
+      </c>
+      <c r="F184" t="n">
+        <v>0.378</v>
+      </c>
+      <c r="G184" t="n">
+        <v>80.31999999999999</v>
+      </c>
+      <c r="H184" t="n">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Empoli</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Verona</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>1</v>
+      </c>
+      <c r="D185" t="n">
+        <v>1</v>
+      </c>
+      <c r="E185" t="n">
+        <v>2.033</v>
+      </c>
+      <c r="F185" t="n">
+        <v>3.428</v>
+      </c>
+      <c r="G185" t="n">
+        <v>14.88</v>
+      </c>
+      <c r="H185" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Venezia</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Sampdoria</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>0</v>
+      </c>
+      <c r="D186" t="n">
+        <v>2</v>
+      </c>
+      <c r="E186" t="n">
+        <v>1.295</v>
+      </c>
+      <c r="F186" t="n">
+        <v>1.598</v>
+      </c>
+      <c r="G186" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="H186" t="n">
+        <v>7.1</v>
       </c>
     </row>
   </sheetData>
@@ -26355,7 +28635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H152"/>
+  <dimension ref="A1:H171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30935,6 +33215,576 @@
         <v>4.8</v>
       </c>
     </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Troyes</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Nantes</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>1</v>
+      </c>
+      <c r="D153" t="n">
+        <v>0</v>
+      </c>
+      <c r="E153" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="F153" t="n">
+        <v>0.863</v>
+      </c>
+      <c r="G153" t="n">
+        <v>30.29</v>
+      </c>
+      <c r="H153" t="n">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Montpellier</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Nice</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>0</v>
+      </c>
+      <c r="D154" t="n">
+        <v>0</v>
+      </c>
+      <c r="E154" t="n">
+        <v>0.676</v>
+      </c>
+      <c r="F154" t="n">
+        <v>1.827</v>
+      </c>
+      <c r="G154" t="n">
+        <v>21.88</v>
+      </c>
+      <c r="H154" t="n">
+        <v>8.199999999999999</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Brest</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Marsylia</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>1</v>
+      </c>
+      <c r="D155" t="n">
+        <v>4</v>
+      </c>
+      <c r="E155" t="n">
+        <v>0.8070000000000001</v>
+      </c>
+      <c r="F155" t="n">
+        <v>1.686</v>
+      </c>
+      <c r="G155" t="n">
+        <v>58.3</v>
+      </c>
+      <c r="H155" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Lyon</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Rennes</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>2</v>
+      </c>
+      <c r="D156" t="n">
+        <v>4</v>
+      </c>
+      <c r="E156" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="F156" t="n">
+        <v>1.413</v>
+      </c>
+      <c r="G156" t="n">
+        <v>36.69</v>
+      </c>
+      <c r="H156" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Strasbourg</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Monaco</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>1</v>
+      </c>
+      <c r="D157" t="n">
+        <v>0</v>
+      </c>
+      <c r="E157" t="n">
+        <v>1.741</v>
+      </c>
+      <c r="F157" t="n">
+        <v>0.945</v>
+      </c>
+      <c r="G157" t="n">
+        <v>56.12</v>
+      </c>
+      <c r="H157" t="n">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Metz</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Lens</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>0</v>
+      </c>
+      <c r="D158" t="n">
+        <v>0</v>
+      </c>
+      <c r="E158" t="n">
+        <v>1.432</v>
+      </c>
+      <c r="F158" t="n">
+        <v>2.506</v>
+      </c>
+      <c r="G158" t="n">
+        <v>18.37</v>
+      </c>
+      <c r="H158" t="n">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Clermont</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Lorient</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>0</v>
+      </c>
+      <c r="D159" t="n">
+        <v>2</v>
+      </c>
+      <c r="E159" t="n">
+        <v>1.545</v>
+      </c>
+      <c r="F159" t="n">
+        <v>0.9409999999999999</v>
+      </c>
+      <c r="G159" t="n">
+        <v>23</v>
+      </c>
+      <c r="H159" t="n">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Angers</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Reims</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>0</v>
+      </c>
+      <c r="D160" t="n">
+        <v>1</v>
+      </c>
+      <c r="E160" t="n">
+        <v>1.042</v>
+      </c>
+      <c r="F160" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="G160" t="n">
+        <v>37.57</v>
+      </c>
+      <c r="H160" t="n">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Bordeaux</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>3</v>
+      </c>
+      <c r="D161" t="n">
+        <v>0</v>
+      </c>
+      <c r="E161" t="n">
+        <v>4.997</v>
+      </c>
+      <c r="F161" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="G161" t="n">
+        <v>95.78</v>
+      </c>
+      <c r="H161" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>St. Etienne</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Troyes</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>1</v>
+      </c>
+      <c r="D162" t="n">
+        <v>1</v>
+      </c>
+      <c r="E162" t="n">
+        <v>1.808</v>
+      </c>
+      <c r="F162" t="n">
+        <v>1.635</v>
+      </c>
+      <c r="G162" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="H162" t="n">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Nantes</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Lille</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>0</v>
+      </c>
+      <c r="D163" t="n">
+        <v>1</v>
+      </c>
+      <c r="E163" t="n">
+        <v>1.669</v>
+      </c>
+      <c r="F163" t="n">
+        <v>1.071</v>
+      </c>
+      <c r="G163" t="n">
+        <v>24.36</v>
+      </c>
+      <c r="H163" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Lens</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Clermont</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>3</v>
+      </c>
+      <c r="D164" t="n">
+        <v>1</v>
+      </c>
+      <c r="E164" t="n">
+        <v>2.498</v>
+      </c>
+      <c r="F164" t="n">
+        <v>0.955</v>
+      </c>
+      <c r="G164" t="n">
+        <v>71</v>
+      </c>
+      <c r="H164" t="n">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Marsylia</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Nice</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>2</v>
+      </c>
+      <c r="D165" t="n">
+        <v>1</v>
+      </c>
+      <c r="E165" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="F165" t="n">
+        <v>1.466</v>
+      </c>
+      <c r="G165" t="n">
+        <v>13.15</v>
+      </c>
+      <c r="H165" t="n">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Reims</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Lyon</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>0</v>
+      </c>
+      <c r="D166" t="n">
+        <v>0</v>
+      </c>
+      <c r="E166" t="n">
+        <v>1.438</v>
+      </c>
+      <c r="F166" t="n">
+        <v>1.129</v>
+      </c>
+      <c r="G166" t="n">
+        <v>26.21</v>
+      </c>
+      <c r="H166" t="n">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Rennes</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Metz</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>6</v>
+      </c>
+      <c r="D167" t="n">
+        <v>1</v>
+      </c>
+      <c r="E167" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="F167" t="n">
+        <v>0.405</v>
+      </c>
+      <c r="G167" t="n">
+        <v>83.53</v>
+      </c>
+      <c r="H167" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Lorient</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Strasbourg</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>0</v>
+      </c>
+      <c r="D168" t="n">
+        <v>0</v>
+      </c>
+      <c r="E168" t="n">
+        <v>0.8179999999999999</v>
+      </c>
+      <c r="F168" t="n">
+        <v>1.687</v>
+      </c>
+      <c r="G168" t="n">
+        <v>23.98</v>
+      </c>
+      <c r="H168" t="n">
+        <v>8.199999999999999</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Bordeaux</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Montpellier</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>0</v>
+      </c>
+      <c r="D169" t="n">
+        <v>2</v>
+      </c>
+      <c r="E169" t="n">
+        <v>1.675</v>
+      </c>
+      <c r="F169" t="n">
+        <v>2.272</v>
+      </c>
+      <c r="G169" t="n">
+        <v>51.43</v>
+      </c>
+      <c r="H169" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Angers</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Brest</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>1</v>
+      </c>
+      <c r="D170" t="n">
+        <v>0</v>
+      </c>
+      <c r="E170" t="n">
+        <v>1.057</v>
+      </c>
+      <c r="F170" t="n">
+        <v>1.306</v>
+      </c>
+      <c r="G170" t="n">
+        <v>30.11</v>
+      </c>
+      <c r="H170" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Monaco</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>3</v>
+      </c>
+      <c r="D171" t="n">
+        <v>0</v>
+      </c>
+      <c r="E171" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="F171" t="n">
+        <v>1.505</v>
+      </c>
+      <c r="G171" t="n">
+        <v>40.87</v>
+      </c>
+      <c r="H171" t="n">
+        <v>3.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>